<commit_message>
Added mapping to CV terms based on Goslin shorthand level.
</commit_message>
<xml_diff>
--- a/inst/extdata/shorthand_cv_map.xlsx
+++ b/inst/extdata/shorthand_cv_map.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="cv_term_map" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+  <si>
+    <t xml:space="preserve">Shorthand.Level</t>
+  </si>
   <si>
     <t xml:space="preserve">ShorthandNomenclatureLevel</t>
   </si>
@@ -31,6 +34,9 @@
     <t xml:space="preserve">CVTermName</t>
   </si>
   <si>
+    <t xml:space="preserve">CATEGORY</t>
+  </si>
+  <si>
     <t xml:space="preserve">Category</t>
   </si>
   <si>
@@ -40,6 +46,9 @@
     <t xml:space="preserve">Lipid shorthand identification confidence – Category</t>
   </si>
   <si>
+    <t xml:space="preserve">CLASS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Class</t>
   </si>
   <si>
@@ -49,6 +58,9 @@
     <t xml:space="preserve">Lipid shorthand identification confidence – Class</t>
   </si>
   <si>
+    <t xml:space="preserve">SPECIES</t>
+  </si>
+  <si>
     <t xml:space="preserve">Species</t>
   </si>
   <si>
@@ -58,6 +70,9 @@
     <t xml:space="preserve">Lipid shorthand identification confidence – Species</t>
   </si>
   <si>
+    <t xml:space="preserve">PHOSPHATE_POSITION</t>
+  </si>
+  <si>
     <t xml:space="preserve">Phosphate-position</t>
   </si>
   <si>
@@ -67,6 +82,9 @@
     <t xml:space="preserve">Lipid shorthand identification confidence – Phosphate-position</t>
   </si>
   <si>
+    <t xml:space="preserve">MOLECULAR_SPECIES</t>
+  </si>
+  <si>
     <t xml:space="preserve">Molecular species</t>
   </si>
   <si>
@@ -76,6 +94,9 @@
     <t xml:space="preserve">Lipid shorthand identification confidence - Molecular species</t>
   </si>
   <si>
+    <t xml:space="preserve">SN_POSITION</t>
+  </si>
+  <si>
     <t xml:space="preserve">sn-position</t>
   </si>
   <si>
@@ -85,6 +106,9 @@
     <t xml:space="preserve">Lipid shorthand identification confidence – sn-position</t>
   </si>
   <si>
+    <t xml:space="preserve">DBE_POSITION</t>
+  </si>
+  <si>
     <t xml:space="preserve">DBE position</t>
   </si>
   <si>
@@ -94,6 +118,9 @@
     <t xml:space="preserve">Lipid shorthand identification confidence - DBE pos</t>
   </si>
   <si>
+    <t xml:space="preserve">STRUCTURE_DEFINED</t>
+  </si>
+  <si>
     <t xml:space="preserve">Structure defined</t>
   </si>
   <si>
@@ -103,6 +130,9 @@
     <t xml:space="preserve">Lipid shorthand identification confidence - Structure defined</t>
   </si>
   <si>
+    <t xml:space="preserve">FULL_STRUCTURE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Full structure</t>
   </si>
   <si>
@@ -110,6 +140,9 @@
   </si>
   <si>
     <t xml:space="preserve">Lipid shorthand identification confidence - Full structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMPLETE_STRUCTURE</t>
   </si>
   <si>
     <t xml:space="preserve">Complete structure</t>
@@ -133,6 +166,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -214,15 +248,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="38.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -235,115 +269,148 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>29</v>
+        <v>38</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>32</v>
+        <v>42</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>